<commit_message>
Update results excel table formulas
</commit_message>
<xml_diff>
--- a/Trade Results.xlsx
+++ b/Trade Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\AASMA_Trade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1396D2BE-CAA8-43EE-AAB7-17ADD21C13E3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EC3E72-01EB-410D-8CE8-D5D55DDD5812}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="815" xr2:uid="{828DDF07-CED7-42D5-9BB2-34513490F6FB}"/>
   </bookViews>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="10">
   <si>
     <t>Column1</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>Average Profit Amount:</t>
+  </si>
+  <si>
+    <t>Column4</t>
   </si>
 </sst>
 </file>
@@ -214,7 +217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -224,6 +227,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -378,11 +382,12 @@
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DadosExternos_6" connectionId="17" xr16:uid="{B61E25E8-E7DB-4987-B901-3D55BBD77E7A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="4">
-    <queryTableFields count="3">
+  <queryTableRefresh nextId="5" unboundColumnsRight="1">
+    <queryTableFields count="4">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
       <queryTableField id="2" name="Column2" tableColumnId="2"/>
       <queryTableField id="3" name="Column3" tableColumnId="3"/>
+      <queryTableField id="4" dataBound="0" tableColumnId="4"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
@@ -617,12 +622,13 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{85A5C721-E7B9-4FA3-AC39-465589FD5BAF}" name="TradeResults6" displayName="TradeResults6" ref="A1:C151" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C151" xr:uid="{860BA4E6-0046-4544-A7A8-1320F1551937}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{85A5C721-E7B9-4FA3-AC39-465589FD5BAF}" name="TradeResults6" displayName="TradeResults6" ref="A1:D151" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D151" xr:uid="{860BA4E6-0046-4544-A7A8-1320F1551937}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D52EACCC-F2E5-4E21-9E4F-ACADBBCC6E7E}" uniqueName="1" name="Column1" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{B01172F0-568F-489C-8B78-690ADCD26A2D}" uniqueName="2" name="Column2" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{85410E71-F874-47D5-B8B8-E8FE3FABAF00}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="1" dataCellStyle="Percentagem"/>
+    <tableColumn id="4" xr3:uid="{607DB90F-B75E-43EA-91D1-A2C5A4B1F0BB}" uniqueName="4" name="Column4" queryTableFieldId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1084,7 +1090,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1155,9 +1161,9 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
-        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults20[Column1] = TRUE,TradeResults20[Column2]))</f>
-        <v>12.627039705040653</v>
+      <c r="F4" s="6">
+        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults20[Column1] = TRUE,TradeResults20[Column2],0))</f>
+        <v>10.354172558133335</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -1174,8 +1180,8 @@
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <f>_xlfn.STDEV.P(TradeResults20[Column3])</f>
-        <v>0.15874554174800468</v>
+        <f t="array" ref="F5">_xlfn.STDEV.P(IF(TradeResults20[Column1]=TRUE, TradeResults20[Column3]))</f>
+        <v>0.13973501299561816</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -1192,8 +1198,8 @@
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults20[Column3] &gt; 0,TradeResults20[Column3]))</f>
-        <v>8.0817035399461917E-2</v>
+        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults20[Column1]=TRUE, IF(TradeResults20[Column3]&gt;0,TradeResults20[Column3])))</f>
+        <v>8.4240086706652867E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -1209,8 +1215,8 @@
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2">
-        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults20[Column3] &lt; 0,TradeResults20[Column3]))</f>
+      <c r="F7" s="3">
+        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults20[Column1]=TRUE, IF(TradeResults20[Column3]&lt;0,TradeResults20[Column3])))</f>
         <v>3.9522260099429808E-2</v>
       </c>
     </row>
@@ -2811,7 +2817,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2882,9 +2888,9 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
-        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults11[Column1] = TRUE,TradeResults11[Column2]))</f>
-        <v>4.7329710000000027</v>
+      <c r="F4" s="6">
+        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults11[Column1] = TRUE,TradeResults11[Column2],0))</f>
+        <v>2.2087198000000012</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -2901,8 +2907,8 @@
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <f>_xlfn.STDEV.P(TradeResults11[Column3])</f>
-        <v>0.1349642554798611</v>
+        <f t="array" ref="F5">_xlfn.STDEV.P(IF(TradeResults11[Column1]=TRUE, TradeResults11[Column3]))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -2919,8 +2925,8 @@
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults11[Column3] &gt; 0,TradeResults11[Column3]))</f>
-        <v>0.1349642554798611</v>
+        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults11[Column1]=TRUE, IF(TradeResults11[Column3]&gt;0,TradeResults11[Column3])))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -2936,8 +2942,8 @@
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2" t="e">
-        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults11[Column3] &lt; 0,TradeResults11[Column3]))</f>
+      <c r="F7" s="3" t="e">
+        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults11[Column1]=TRUE, IF(TradeResults11[Column3]&lt;0,TradeResults11[Column3])))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4538,7 +4544,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4547,6 +4553,7 @@
     <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -4609,9 +4616,9 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
-        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults10[Column1] = TRUE,TradeResults10[Column2]))</f>
-        <v>48.317437499999969</v>
+      <c r="F4" s="6">
+        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults10[Column1] = TRUE,TradeResults10[Column2],0))</f>
+        <v>27.057764999999982</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -4628,8 +4635,8 @@
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <f>_xlfn.STDEV.P(TradeResults10[Column3])</f>
-        <v>0.14133868775681993</v>
+        <f t="array" ref="F5">_xlfn.STDEV.P(IF(TradeResults10[Column1]=TRUE, TradeResults10[Column3]))</f>
+        <v>1.8652208079980838E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -4646,8 +4653,8 @@
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults10[Column3] &gt; 0,TradeResults10[Column3]))</f>
-        <v>0.14133868775681993</v>
+        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults10[Column1]=TRUE, IF(TradeResults10[Column3]&gt;0,TradeResults10[Column3])))</f>
+        <v>1.8652208079980838E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -4663,9 +4670,9 @@
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2">
-        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults3[Column3] &lt; 0,TradeResults3[Column3]))</f>
-        <v>1.3877787807814457E-16</v>
+      <c r="F7" s="3" t="e">
+        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults10[Column1]=TRUE, IF(TradeResults10[Column3]&lt;0,TradeResults10[Column3])))</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -6265,7 +6272,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6336,9 +6343,9 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
-        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults9[Column1] = TRUE,TradeResults9[Column2]))</f>
-        <v>4.7329710000000045</v>
+      <c r="F4" s="6">
+        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults9[Column1] = TRUE,TradeResults9[Column2],0))</f>
+        <v>2.4295917800000022</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -6355,8 +6362,8 @@
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <f>_xlfn.STDEV.P(TradeResults9[Column3])</f>
-        <v>0.17194866457114508</v>
+        <f t="array" ref="F5">_xlfn.STDEV.P(IF(TradeResults9[Column1]=TRUE, TradeResults9[Column3]))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -6373,8 +6380,8 @@
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults9[Column3] &gt; 0,TradeResults9[Column3]))</f>
-        <v>0.17194866457114508</v>
+        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults9[Column1]=TRUE, IF(TradeResults9[Column3]&gt;0,TradeResults9[Column3])))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -6390,8 +6397,8 @@
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2" t="e">
-        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults9[Column3] &lt; 0,TradeResults9[Column3]))</f>
+      <c r="F7" s="3" t="e">
+        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults9[Column1]=TRUE, IF(TradeResults9[Column3]&lt;0,TradeResults9[Column3])))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7992,7 +7999,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8063,8 +8070,8 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
-        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults8[Column1] = TRUE,TradeResults8[Column2]))</f>
+      <c r="F4" s="6">
+        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults8[Column1] = TRUE,TradeResults8[Column2],0))</f>
         <v>-22.228775611333308</v>
       </c>
     </row>
@@ -8082,7 +8089,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <f>_xlfn.STDEV.P(TradeResults8[Column3])</f>
+        <f t="array" ref="F5">_xlfn.STDEV.P(IF(TradeResults8[Column1]=TRUE, TradeResults8[Column3]))</f>
         <v>0.10238522678065584</v>
       </c>
     </row>
@@ -8100,7 +8107,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults8[Column3] &gt; 0,TradeResults8[Column3]))</f>
+        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults8[Column1]=TRUE, IF(TradeResults8[Column3]&gt;0,TradeResults8[Column3])))</f>
         <v>4.2352237372945717E-2</v>
       </c>
     </row>
@@ -8118,7 +8125,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="3">
-        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults8[Column3] &lt; 0,TradeResults8[Column3]))</f>
+        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults8[Column1]=TRUE, IF(TradeResults8[Column3]&lt;0,TradeResults8[Column3])))</f>
         <v>5.3329281326144312E-2</v>
       </c>
     </row>
@@ -9719,7 +9726,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9728,6 +9735,7 @@
     <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -9790,9 +9798,9 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
-        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults7[Column1] = TRUE,TradeResults7[Column2]))</f>
-        <v>26.845702999999972</v>
+      <c r="F4" s="6">
+        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults7[Column1] = TRUE,TradeResults7[Column2],0))</f>
+        <v>13.243880146666653</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -9809,8 +9817,8 @@
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <f>_xlfn.STDEV.P(TradeResults7[Column3])</f>
-        <v>0.13397546948128658</v>
+        <f t="array" ref="F5">_xlfn.STDEV.P(IF(TradeResults7[Column1]=TRUE, TradeResults7[Column3]))</f>
+        <v>1.3877787807814457E-17</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -9827,7 +9835,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults7[Column3] &gt; 0,TradeResults7[Column3]))</f>
+        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults7[Column1]=TRUE, IF(TradeResults7[Column3]&gt;0,TradeResults7[Column3])))</f>
         <v>1.3877787807814457E-17</v>
       </c>
     </row>
@@ -9844,9 +9852,9 @@
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="3">
-        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults7[Column3] &lt; 0,TradeResults7[Column3]))</f>
-        <v>3.0531133177191805E-16</v>
+      <c r="F7" s="3" t="e">
+        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults7[Column1]=TRUE, IF(TradeResults7[Column3]&lt;0,TradeResults7[Column3])))</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -11446,7 +11454,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11454,7 +11462,9 @@
     <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" customWidth="1"/>
     <col min="5" max="5" width="29.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -11467,6 +11477,9 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" t="b">
@@ -11514,11 +11527,14 @@
       <c r="C4" s="2">
         <v>0.17599766999999999</v>
       </c>
+      <c r="D4" s="2">
+        <v>0.17599766999999999</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
-        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults6[Column1] = TRUE,TradeResults6[Column2]))</f>
+      <c r="F4" s="6">
+        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults6[Column1] = TRUE,TradeResults6[Column2],0))</f>
         <v>-2.3711962266666666</v>
       </c>
     </row>
@@ -11532,11 +11548,14 @@
       <c r="C5" s="2">
         <v>0.11024365</v>
       </c>
+      <c r="D5" s="2">
+        <v>0.11024365</v>
+      </c>
       <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <f>_xlfn.STDEV.P(TradeResults6[Column3])</f>
+        <f>_xlfn.STDEV.P(IF(TradeResults6[Column1]=TRUE, TradeResults6[Column3]))</f>
         <v>0.13038675212501014</v>
       </c>
     </row>
@@ -11554,7 +11573,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults6[Column3] &gt; 0,TradeResults6[Column3]))</f>
+        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults6[Column1]=TRUE, IF(TradeResults6[Column3]&gt;0,TradeResults6[Column3])))</f>
         <v>3.6394049271419628E-2</v>
       </c>
     </row>
@@ -11572,7 +11591,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="3">
-        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults6[Column3] &lt; 0,TradeResults6[Column3]))</f>
+        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults6[Column1]=TRUE, IF(TradeResults6[Column3]&lt;0,TradeResults6[Column3])))</f>
         <v>5.4922715541288553E-2</v>
       </c>
     </row>
@@ -11586,6 +11605,9 @@
       <c r="C8" s="2">
         <v>0.15781893999999999</v>
       </c>
+      <c r="D8" s="2">
+        <v>0.15781893999999999</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="b">
@@ -11597,6 +11619,9 @@
       <c r="C9" s="2">
         <v>0.15469791999999999</v>
       </c>
+      <c r="D9" s="2">
+        <v>0.15469791999999999</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="b">
@@ -11608,6 +11633,13 @@
       <c r="C10" s="2">
         <v>8.2407380000000002E-2</v>
       </c>
+      <c r="D10" s="2">
+        <v>8.2407380000000002E-2</v>
+      </c>
+      <c r="F10" s="5">
+        <f>_xlfn.STDEV.P(D4:D5,D8:D10,D12:D14,D17:D18)</f>
+        <v>3.7833021243089494E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="b">
@@ -11630,6 +11662,9 @@
       <c r="C12" s="2">
         <v>0.11751158</v>
       </c>
+      <c r="D12" s="2">
+        <v>0.11751158</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="b">
@@ -11641,6 +11676,9 @@
       <c r="C13" s="2">
         <v>0.18413475000000001</v>
       </c>
+      <c r="D13" s="2">
+        <v>0.18413475000000001</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="b">
@@ -11652,6 +11690,9 @@
       <c r="C14" s="2">
         <v>8.2407380000000002E-2</v>
       </c>
+      <c r="D14" s="2">
+        <v>8.2407380000000002E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="b">
@@ -11675,7 +11716,7 @@
         <v>-0.16929135000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="b">
         <v>1</v>
       </c>
@@ -11685,8 +11726,11 @@
       <c r="C17" s="2">
         <v>0.18044432999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" s="2">
+        <v>0.18044432999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="b">
         <v>1</v>
       </c>
@@ -11696,8 +11740,11 @@
       <c r="C18" s="2">
         <v>0.16999868000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" s="2">
+        <v>0.16999868000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="b">
         <v>1</v>
       </c>
@@ -11708,7 +11755,7 @@
         <v>-0.12512240999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="b">
         <v>1</v>
       </c>
@@ -11719,7 +11766,7 @@
         <v>-7.7819063999999993E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="b">
         <v>1</v>
       </c>
@@ -11730,7 +11777,7 @@
         <v>-0.16929135000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="b">
         <v>1</v>
       </c>
@@ -11741,7 +11788,7 @@
         <v>0.12187051</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="b">
         <v>1</v>
       </c>
@@ -11752,7 +11799,7 @@
         <v>-0.15826916999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="b">
         <v>1</v>
       </c>
@@ -11763,7 +11810,7 @@
         <v>-0.16929135000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="b">
         <v>1</v>
       </c>
@@ -11774,7 +11821,7 @@
         <v>-8.1650630000000002E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="b">
         <v>1</v>
       </c>
@@ -11785,7 +11832,7 @@
         <v>-0.16929135000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="b">
         <v>1</v>
       </c>
@@ -11795,8 +11842,11 @@
       <c r="C27" s="2">
         <v>0.1340015</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" s="2">
+        <v>0.1340015</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="b">
         <v>1</v>
       </c>
@@ -11806,8 +11856,11 @@
       <c r="C28" s="2">
         <v>-8.6333549999999995E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" s="2">
+        <v>-8.6333549999999995E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="b">
         <v>1</v>
       </c>
@@ -11818,7 +11871,7 @@
         <v>-0.16929135000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="b">
         <v>1</v>
       </c>
@@ -11829,7 +11882,7 @@
         <v>0.11011412</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="b">
         <v>1</v>
       </c>
@@ -11840,7 +11893,7 @@
         <v>8.2407380000000002E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="b">
         <v>1</v>
       </c>
@@ -13173,7 +13226,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13244,9 +13297,9 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
-        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults5[Column1] = TRUE,TradeResults5[Column2]))</f>
-        <v>75.558960000000027</v>
+      <c r="F4" s="6">
+        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults5[Column1] = TRUE,TradeResults5[Column2],0))</f>
+        <v>36.772027200000011</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -13263,8 +13316,8 @@
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <f>_xlfn.STDEV.P(TradeResults5[Column3])</f>
-        <v>0.1677563514668185</v>
+        <f t="array" ref="F5">_xlfn.STDEV.P(IF(TradeResults5[Column1]=TRUE, TradeResults5[Column3]))</f>
+        <v>1.9428902930940239E-16</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -13281,7 +13334,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults5[Column3] &gt; 0,TradeResults5[Column3]))</f>
+        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults5[Column1]=TRUE, IF(TradeResults5[Column3]&gt;0,TradeResults5[Column3])))</f>
         <v>1.9428902930940239E-16</v>
       </c>
     </row>
@@ -13298,9 +13351,9 @@
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="3">
-        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults5[Column3] &lt; 0,TradeResults5[Column3]))</f>
-        <v>3.0531133177191805E-16</v>
+      <c r="F7" s="3" t="e">
+        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults5[Column1]=TRUE, IF(TradeResults5[Column3]&lt;0,TradeResults5[Column3])))</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -14901,7 +14954,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14972,8 +15025,8 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
-        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults4[Column1] = TRUE,TradeResults4[Column2]))</f>
+      <c r="F4" s="6">
+        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults4[Column1] = TRUE,TradeResults4[Column2],0))</f>
         <v>48.464078896066653</v>
       </c>
     </row>
@@ -14991,7 +15044,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <f>_xlfn.STDEV.P(TradeResults4[Column3])</f>
+        <f t="array" ref="F5">_xlfn.STDEV.P(IF(TradeResults4[Column1]=TRUE, TradeResults4[Column3]))</f>
         <v>9.0273548882788712E-2</v>
       </c>
     </row>
@@ -15009,7 +15062,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults4[Column3] &gt; 0,TradeResults4[Column3]))</f>
+        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults4[Column1]=TRUE, IF(TradeResults4[Column3]&gt;0,TradeResults4[Column3])))</f>
         <v>6.6346347016548152E-2</v>
       </c>
     </row>
@@ -15027,7 +15080,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="3">
-        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults4[Column3] &lt; 0,TradeResults4[Column3]))</f>
+        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults4[Column1]=TRUE, IF(TradeResults4[Column3]&lt;0,TradeResults4[Column3])))</f>
         <v>1.7851288480717653E-2</v>
       </c>
     </row>
@@ -16628,7 +16681,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16700,8 +16753,8 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
-        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults3[Column1] = TRUE,TradeResults3[Column2]))</f>
+      <c r="F4" s="6">
+        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults3[Column1] = TRUE,TradeResults3[Column2],0))</f>
         <v>21.719849519999958</v>
       </c>
     </row>
@@ -16719,7 +16772,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <f>_xlfn.STDEV.P(TradeResults3[Column3])</f>
+        <f t="array" ref="F5">_xlfn.STDEV.P(IF(TradeResults3[Column1]=TRUE, TradeResults3[Column3]))</f>
         <v>0.12178796974600613</v>
       </c>
     </row>
@@ -16737,7 +16790,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults3[Column3] &gt; 0,TradeResults3[Column3]))</f>
+        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults3[Column1]=TRUE, IF(TradeResults3[Column3]&gt;0,TradeResults3[Column3])))</f>
         <v>1.3877787807814457E-16</v>
       </c>
     </row>
@@ -16755,7 +16808,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="3">
-        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults3[Column3] &lt; 0,TradeResults3[Column3]))</f>
+        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults3[Column1]=TRUE, IF(TradeResults3[Column3]&lt;0,TradeResults3[Column3])))</f>
         <v>1.3877787807814457E-16</v>
       </c>
     </row>
@@ -18356,7 +18409,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18428,9 +18481,9 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
-        <f xml:space="preserve"> AVERAGE(IF(TradeResults2[Column1] = TRUE,TradeResults2[Column2]))</f>
-        <v>0</v>
+      <c r="F4" s="6">
+        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults2[Column1] = TRUE,TradeResults2[Column2],0))</f>
+        <v>48.369093368000009</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -18447,8 +18500,8 @@
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <f>_xlfn.STDEV.P(TradeResults2[Column3])</f>
-        <v>0.11814720392569633</v>
+        <f t="array" ref="F5">_xlfn.STDEV.P(IF(TradeResults2[Column1]=TRUE, TradeResults2[Column3]))</f>
+        <v>0.10961245364485935</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -18465,8 +18518,8 @@
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults2[Column3] &gt; 0,TradeResults2[Column3]))</f>
-        <v>9.3119453511761457E-2</v>
+        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults2[Column1]=TRUE, IF(TradeResults2[Column3]&gt;0,TradeResults2[Column3])))</f>
+        <v>8.8026232000923396E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -18483,7 +18536,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="3">
-        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults2[Column3] &lt; 0,TradeResults2[Column3]))</f>
+        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults2[Column1]=TRUE, IF(TradeResults2[Column3]&lt;0,TradeResults2[Column3])))</f>
         <v>1.7207959699966746E-2</v>
       </c>
     </row>
@@ -20084,7 +20137,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20155,9 +20208,9 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
-        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults19[Column1] = TRUE,TradeResults19[Column2]))</f>
-        <v>166.6080299999999</v>
+      <c r="F4" s="6">
+        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults19[Column1] = TRUE,TradeResults19[Column2],0))</f>
+        <v>85.525455399999942</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -20174,8 +20227,8 @@
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <f>_xlfn.STDEV.P(TradeResults19[Column3])</f>
-        <v>0.22962407731427326</v>
+        <f t="array" ref="F5">_xlfn.STDEV.P(IF(TradeResults19[Column1]=TRUE, TradeResults19[Column3]))</f>
+        <v>1.3877787807814457E-16</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -20192,7 +20245,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults19[Column3] &gt; 0,TradeResults19[Column3]))</f>
+        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults19[Column1]=TRUE, IF(TradeResults19[Column3]&gt;0,TradeResults19[Column3])))</f>
         <v>1.3877787807814457E-16</v>
       </c>
     </row>
@@ -20209,9 +20262,9 @@
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2">
-        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults19[Column3] &lt; 0,TradeResults19[Column3]))</f>
-        <v>2.7755575615628914E-17</v>
+      <c r="F7" s="3" t="e">
+        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults19[Column1]=TRUE, IF(TradeResults19[Column3]&lt;0,TradeResults19[Column3])))</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -21811,7 +21864,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21883,8 +21936,8 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
-        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults1[Column1] = TRUE,TradeResults1[Column2]))</f>
+      <c r="F4" s="6">
+        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults1[Column1] = TRUE,TradeResults1[Column2],0))</f>
         <v>44.702387466666686</v>
       </c>
     </row>
@@ -21902,7 +21955,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <f>_xlfn.STDEV.P(TradeResults1[Column3])</f>
+        <f t="array" ref="F5">_xlfn.STDEV.P(IF(TradeResults1[Column1]=TRUE, TradeResults1[Column3]))</f>
         <v>0.15704719136940226</v>
       </c>
     </row>
@@ -21920,7 +21973,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults1[Column3] &gt; 0,TradeResults1[Column3]))</f>
+        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults1[Column1]=TRUE, IF(TradeResults1[Column3]&gt;0,TradeResults1[Column3])))</f>
         <v>2.4980018054066022E-16</v>
       </c>
     </row>
@@ -21938,7 +21991,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="3">
-        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults1[Column3] &lt; 0,TradeResults1[Column3]))</f>
+        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults1[Column1]=TRUE, IF(TradeResults1[Column3]&lt;0,TradeResults1[Column3])))</f>
         <v>1.5265566588595902E-16</v>
       </c>
     </row>
@@ -23540,7 +23593,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23611,9 +23664,9 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
-        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults18[Column1] = TRUE,TradeResults18[Column2]))</f>
-        <v>-56.013082057464821</v>
+      <c r="F4" s="6">
+        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults18[Column1] = TRUE,TradeResults18[Column2],0))</f>
+        <v>-26.512858840533347</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -23630,8 +23683,8 @@
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <f>_xlfn.STDEV.P(TradeResults18[Column3])</f>
-        <v>0.21224242709070792</v>
+        <f t="array" ref="F5">_xlfn.STDEV.P(IF(TradeResults18[Column1]=TRUE, TradeResults18[Column3]))</f>
+        <v>5.0196867369223075E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -23648,8 +23701,8 @@
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults18[Column3] &gt; 0,TradeResults18[Column3]))</f>
-        <v>9.1466426925121844E-2</v>
+        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults18[Column1]=TRUE, IF(TradeResults18[Column3]&gt;0,TradeResults18[Column3])))</f>
+        <v>9.3539250523233773E-3</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -23665,8 +23718,8 @@
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2">
-        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults18[Column3] &lt; 0,TradeResults18[Column3]))</f>
+      <c r="F7" s="3">
+        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults18[Column1]=TRUE, IF(TradeResults18[Column3]&lt;0,TradeResults18[Column3])))</f>
         <v>4.1257089168497775E-2</v>
       </c>
     </row>
@@ -25267,7 +25320,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25337,9 +25390,9 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5" t="e">
-        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults17[Column1] = TRUE,TradeResults17[Column2]))</f>
-        <v>#DIV/0!</v>
+      <c r="F4" s="6">
+        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults17[Column1] = TRUE,TradeResults17[Column2],0))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -25355,9 +25408,9 @@
       <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="2">
-        <f>_xlfn.STDEV.P(TradeResults17[Column3])</f>
-        <v>0.286046339996326</v>
+      <c r="F5" s="2" t="e">
+        <f t="array" ref="F5">_xlfn.STDEV.P(IF(TradeResults17[Column1]=TRUE, TradeResults17[Column3]))</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -25373,9 +25426,9 @@
       <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="2">
-        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults17[Column3] &gt; 0,TradeResults17[Column3]))</f>
-        <v>5.5511151231257827E-17</v>
+      <c r="F6" s="2" t="e">
+        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults17[Column1]=TRUE, IF(TradeResults17[Column3]&gt;0,TradeResults17[Column3])))</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -25391,9 +25444,9 @@
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2">
-        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults17[Column3] &lt; 0,TradeResults17[Column3]))</f>
-        <v>2.7755575615628914E-17</v>
+      <c r="F7" s="3" t="e">
+        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults17[Column1]=TRUE, IF(TradeResults17[Column3]&lt;0,TradeResults17[Column3])))</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -26993,7 +27046,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27064,8 +27117,8 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
-        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults16[Column1] = TRUE,TradeResults16[Column2]))</f>
+      <c r="F4" s="6">
+        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults16[Column1] = TRUE,TradeResults16[Column2],0))</f>
         <v>27.87105378033333</v>
       </c>
     </row>
@@ -27083,7 +27136,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <f>_xlfn.STDEV.P(TradeResults16[Column3])</f>
+        <f t="array" ref="F5">_xlfn.STDEV.P(IF(TradeResults16[Column1]=TRUE, TradeResults16[Column3]))</f>
         <v>5.4497773914530569E-2</v>
       </c>
     </row>
@@ -27101,7 +27154,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults16[Column3] &gt; 0,TradeResults16[Column3]))</f>
+        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults16[Column1]=TRUE, IF(TradeResults16[Column3]&gt;0,TradeResults16[Column3])))</f>
         <v>3.9119825396418173E-2</v>
       </c>
     </row>
@@ -27118,8 +27171,8 @@
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2">
-        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults16[Column3] &lt; 0,TradeResults16[Column3]))</f>
+      <c r="F7" s="3">
+        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults16[Column1]=TRUE, IF(TradeResults16[Column3]&lt;0,TradeResults16[Column3])))</f>
         <v>1.3229654794013329E-2</v>
       </c>
     </row>
@@ -28720,7 +28773,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28791,8 +28844,8 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
-        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults15[Column1] = TRUE,TradeResults15[Column2]))</f>
+      <c r="F4" s="6">
+        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults15[Column1] = TRUE,TradeResults15[Column2],0))</f>
         <v>4.0140182666666488</v>
       </c>
     </row>
@@ -28810,7 +28863,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <f>_xlfn.STDEV.P(TradeResults15[Column3])</f>
+        <f t="array" ref="F5">_xlfn.STDEV.P(IF(TradeResults15[Column1]=TRUE, TradeResults15[Column3]))</f>
         <v>7.7639510009708007E-2</v>
       </c>
     </row>
@@ -28828,7 +28881,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults15[Column3] &gt; 0,TradeResults15[Column3]))</f>
+        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults15[Column1]=TRUE, IF(TradeResults15[Column3]&gt;0,TradeResults15[Column3])))</f>
         <v>0</v>
       </c>
     </row>
@@ -28845,8 +28898,8 @@
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2">
-        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults15[Column3] &lt; 0,TradeResults15[Column3]))</f>
+      <c r="F7" s="3">
+        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults15[Column1]=TRUE, IF(TradeResults15[Column3]&lt;0,TradeResults15[Column3])))</f>
         <v>6.9388939039072284E-17</v>
       </c>
     </row>
@@ -30447,7 +30500,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30518,8 +30571,8 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
-        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults14[Column1] = TRUE,TradeResults14[Column2]))</f>
+      <c r="F4" s="6">
+        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults14[Column1] = TRUE,TradeResults14[Column2],0))</f>
         <v>49.659109601733363</v>
       </c>
     </row>
@@ -30537,7 +30590,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <f>_xlfn.STDEV.P(TradeResults14[Column3])</f>
+        <f t="array" ref="F5">_xlfn.STDEV.P(IF(TradeResults14[Column1]=TRUE, TradeResults14[Column3]))</f>
         <v>8.0714971248515163E-2</v>
       </c>
     </row>
@@ -30555,7 +30608,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults14[Column3] &gt; 0,TradeResults14[Column3]))</f>
+        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults14[Column1]=TRUE, IF(TradeResults14[Column3]&gt;0,TradeResults14[Column3])))</f>
         <v>6.2541127931860729E-2</v>
       </c>
     </row>
@@ -30572,8 +30625,8 @@
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2">
-        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults14[Column3] &lt; 0,TradeResults14[Column3]))</f>
+      <c r="F7" s="3">
+        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults14[Column1]=TRUE, IF(TradeResults14[Column3]&lt;0,TradeResults14[Column3])))</f>
         <v>1.2612795533327358E-2</v>
       </c>
     </row>
@@ -32245,8 +32298,8 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
-        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults13[Column1] = TRUE,TradeResults13[Column2]))</f>
+      <c r="F4" s="6">
+        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults13[Column1] = TRUE,TradeResults13[Column2],0))</f>
         <v>16.514801306666726</v>
       </c>
     </row>
@@ -32264,7 +32317,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <f>_xlfn.STDEV.P(TradeResults13[Column3])</f>
+        <f t="array" ref="F5">_xlfn.STDEV.P(IF(TradeResults13[Column1]=TRUE, TradeResults13[Column3]))</f>
         <v>9.8817474451127998E-2</v>
       </c>
     </row>
@@ -32282,7 +32335,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults13[Column3] &gt; 0,TradeResults13[Column3]))</f>
+        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults13[Column1]=TRUE, IF(TradeResults13[Column3]&gt;0,TradeResults13[Column3])))</f>
         <v>5.5511151231257827E-17</v>
       </c>
     </row>
@@ -32299,8 +32352,8 @@
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2">
-        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults13[Column3] &lt; 0,TradeResults13[Column3]))</f>
+      <c r="F7" s="3">
+        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults13[Column1]=TRUE, IF(TradeResults13[Column3]&lt;0,TradeResults13[Column3])))</f>
         <v>6.9388939039072284E-17</v>
       </c>
     </row>
@@ -33901,7 +33954,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33972,9 +34025,9 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
-        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults12[Column1] = TRUE,TradeResults12[Column2]))</f>
-        <v>71.329282222069068</v>
+      <c r="F4" s="6">
+        <f t="array" ref="F4" xml:space="preserve"> AVERAGE(IF(TradeResults12[Column1] = TRUE,TradeResults12[Column2],0))</f>
+        <v>68.95163948133343</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -33991,8 +34044,8 @@
         <v>5</v>
       </c>
       <c r="F5" s="2">
-        <f>_xlfn.STDEV.P(TradeResults12[Column3])</f>
-        <v>8.1557227607386554E-2</v>
+        <f t="array" ref="F5">_xlfn.STDEV.P(IF(TradeResults12[Column1]=TRUE, TradeResults12[Column3]))</f>
+        <v>7.6077245945349675E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -34009,8 +34062,8 @@
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults12[Column3] &gt; 0,TradeResults12[Column3]))</f>
-        <v>8.1557227607386554E-2</v>
+        <f t="array" ref="F6">_xlfn.STDEV.P(IF(TradeResults12[Column1]=TRUE, IF(TradeResults12[Column3]&gt;0,TradeResults12[Column3])))</f>
+        <v>7.6077245945349675E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -34026,8 +34079,8 @@
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2" t="e">
-        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults12[Column3] &lt; 0,TradeResults12[Column3]))</f>
+      <c r="F7" s="3" t="e">
+        <f t="array" ref="F7">_xlfn.STDEV.P(IF(TradeResults12[Column1]=TRUE, IF(TradeResults12[Column3]&lt;0,TradeResults12[Column3])))</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>